<commit_message>
Add new Excel reader class
</commit_message>
<xml_diff>
--- a/TestData/New XLSX Worksheet.xlsx
+++ b/TestData/New XLSX Worksheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="22188" windowHeight="9000"/>
+    <workbookView windowWidth="16860" windowHeight="7055"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
   <si>
     <t>Column-1</t>
   </si>
@@ -196,6 +196,9 @@
   </si>
   <si>
     <t>G8</t>
+  </si>
+  <si>
+    <t>Hello</t>
   </si>
 </sst>
 </file>
@@ -1133,7 +1136,7 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="7" outlineLevelCol="6"/>
@@ -1331,14 +1334,20 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1"/>
+  <dimension ref="A3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4"/>
-  <sheetData/>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="2"/>
+  <sheetData>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>

</xml_diff>

<commit_message>
Add new excel reader class for DocumentFormat.OpenXml
</commit_message>
<xml_diff>
--- a/TestData/New XLSX Worksheet.xlsx
+++ b/TestData/New XLSX Worksheet.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="16860" windowHeight="7055"/>
+    <workbookView windowWidth="22188" windowHeight="9000"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId2"/>
+    <sheet name="Hello1" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -28,177 +29,69 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
-  <si>
-    <t>Column-1</t>
-  </si>
-  <si>
-    <t>Column-2</t>
-  </si>
-  <si>
-    <t>Column-3</t>
-  </si>
-  <si>
-    <t>Column-4</t>
-  </si>
-  <si>
-    <t>Column-5</t>
-  </si>
-  <si>
-    <t>Column-6</t>
-  </si>
-  <si>
-    <t>Column-7</t>
-  </si>
-  <si>
-    <t>A2</t>
-  </si>
-  <si>
-    <t>B2</t>
-  </si>
-  <si>
-    <t>C2</t>
-  </si>
-  <si>
-    <t>D2</t>
-  </si>
-  <si>
-    <t>E2</t>
-  </si>
-  <si>
-    <t>F2</t>
-  </si>
-  <si>
-    <t>G2</t>
-  </si>
-  <si>
-    <t>A3</t>
-  </si>
-  <si>
-    <t>B3</t>
-  </si>
-  <si>
-    <t>C3</t>
-  </si>
-  <si>
-    <t>D3</t>
-  </si>
-  <si>
-    <t>E3</t>
-  </si>
-  <si>
-    <t>F3</t>
-  </si>
-  <si>
-    <t>G3</t>
-  </si>
-  <si>
-    <t>A4</t>
-  </si>
-  <si>
-    <t>B4</t>
-  </si>
-  <si>
-    <t>C4</t>
-  </si>
-  <si>
-    <t>D4</t>
-  </si>
-  <si>
-    <t>E4</t>
-  </si>
-  <si>
-    <t>F4</t>
-  </si>
-  <si>
-    <t>G4</t>
-  </si>
-  <si>
-    <t>A5</t>
-  </si>
-  <si>
-    <t>B5</t>
-  </si>
-  <si>
-    <t>C5</t>
-  </si>
-  <si>
-    <t>D5</t>
-  </si>
-  <si>
-    <t>E5</t>
-  </si>
-  <si>
-    <t>F5</t>
-  </si>
-  <si>
-    <t>G5</t>
-  </si>
-  <si>
-    <t>A6</t>
-  </si>
-  <si>
-    <t>B6</t>
-  </si>
-  <si>
-    <t>C6</t>
-  </si>
-  <si>
-    <t>D6</t>
-  </si>
-  <si>
-    <t>E6</t>
-  </si>
-  <si>
-    <t>F6</t>
-  </si>
-  <si>
-    <t>G6</t>
-  </si>
-  <si>
-    <t>A7</t>
-  </si>
-  <si>
-    <t>B7</t>
-  </si>
-  <si>
-    <t>C7</t>
-  </si>
-  <si>
-    <t>D7</t>
-  </si>
-  <si>
-    <t>E7</t>
-  </si>
-  <si>
-    <t>F7</t>
-  </si>
-  <si>
-    <t>G7</t>
-  </si>
-  <si>
-    <t>A8</t>
-  </si>
-  <si>
-    <t>B8</t>
-  </si>
-  <si>
-    <t>C8</t>
-  </si>
-  <si>
-    <t>D8</t>
-  </si>
-  <si>
-    <t>E8</t>
-  </si>
-  <si>
-    <t>F8</t>
-  </si>
-  <si>
-    <t>G8</t>
-  </si>
-  <si>
-    <t>Hello</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="21">
+  <si>
+    <t>alsdfjdsf1</t>
+  </si>
+  <si>
+    <t>alsdfjdsf2</t>
+  </si>
+  <si>
+    <t>alsdfjdsf3</t>
+  </si>
+  <si>
+    <t>alsdfjdsf4</t>
+  </si>
+  <si>
+    <t>alsdfjdsf5</t>
+  </si>
+  <si>
+    <t>alsdfjdsf6</t>
+  </si>
+  <si>
+    <t>alsdfjdsf7</t>
+  </si>
+  <si>
+    <t>alsdfjdsf8</t>
+  </si>
+  <si>
+    <t>alsdfjdsf9</t>
+  </si>
+  <si>
+    <t>alsdfjdsf10</t>
+  </si>
+  <si>
+    <t>alsdfjdsf11</t>
+  </si>
+  <si>
+    <t>alsdfjdsf12</t>
+  </si>
+  <si>
+    <t>alsdfjdsf13</t>
+  </si>
+  <si>
+    <t>alsdfjdsf14</t>
+  </si>
+  <si>
+    <t>alsdfjdsf15</t>
+  </si>
+  <si>
+    <t>alsdfjdsf16</t>
+  </si>
+  <si>
+    <t>alsdfjdsf17</t>
+  </si>
+  <si>
+    <t>alsdfjdsf18</t>
+  </si>
+  <si>
+    <t>hi</t>
+  </si>
+  <si>
+    <t>Shahin</t>
+  </si>
+  <si>
+    <t>Afrin</t>
   </si>
 </sst>
 </file>
@@ -666,7 +559,9 @@
     </border>
   </borders>
   <cellStyleXfs count="49">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -813,7 +708,9 @@
     </xf>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -866,7 +763,221 @@
     <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
     <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="17">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.799981688894314"/>
+          <bgColor theme="4" tint="0.799981688894314"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.799981688894314"/>
+          <bgColor theme="4" tint="0.799981688894314"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="1"/>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="1"/>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="1"/>
+        <color theme="1"/>
+      </font>
+      <border>
+        <top style="double">
+          <color theme="4"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="1"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <border>
+        <left style="thin">
+          <color theme="4"/>
+        </left>
+        <right style="thin">
+          <color theme="4"/>
+        </right>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4"/>
+        </bottom>
+        <horizontal style="thin">
+          <color theme="4" tint="0.399975585192419"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.799981688894314"/>
+          <bgColor theme="4" tint="0.799981688894314"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="4" tint="0.399975585192419"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.799981688894314"/>
+          <bgColor theme="4" tint="0.799981688894314"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="4" tint="0.399975585192419"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <border>
+        <bottom style="thin">
+          <color theme="4" tint="0.399975585192419"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="1"/>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="1"/>
+        <color theme="1"/>
+      </font>
+      <border>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.799981688894314"/>
+          <bgColor theme="4" tint="0.799981688894314"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.799981688894314"/>
+          <bgColor theme="4" tint="0.799981688894314"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="1"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.799981688894314"/>
+          <bgColor theme="4" tint="0.799981688894314"/>
+        </patternFill>
+      </fill>
+      <border>
+        <top style="thin">
+          <color theme="4" tint="0.399975585192419"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.399975585192419"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="1"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.799981688894314"/>
+          <bgColor theme="4" tint="0.799981688894314"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="4" tint="0.399975585192419"/>
+        </bottom>
+      </border>
+    </dxf>
+  </dxfs>
+  <tableStyles count="2" defaultTableStyle="TableStylePreset3_Accent1" defaultPivotStyle="PivotStylePreset2_Accent1">
+    <tableStyle name="TableStylePreset3_Accent1" pivot="0" count="7" xr9:uid="{59DB682C-5494-4EDE-A608-00C9E5F0F923}">
+      <tableStyleElement type="wholeTable" dxfId="6"/>
+      <tableStyleElement type="headerRow" dxfId="5"/>
+      <tableStyleElement type="totalRow" dxfId="4"/>
+      <tableStyleElement type="firstColumn" dxfId="3"/>
+      <tableStyleElement type="lastColumn" dxfId="2"/>
+      <tableStyleElement type="firstRowStripe" dxfId="1"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="0"/>
+    </tableStyle>
+    <tableStyle name="PivotStylePreset2_Accent1" table="0" count="10" xr9:uid="{267968C8-6FFD-4C36-ACC1-9EA1FD1885CA}">
+      <tableStyleElement type="headerRow" dxfId="16"/>
+      <tableStyleElement type="totalRow" dxfId="15"/>
+      <tableStyleElement type="firstRowStripe" dxfId="14"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="13"/>
+      <tableStyleElement type="firstSubtotalRow" dxfId="12"/>
+      <tableStyleElement type="secondSubtotalRow" dxfId="11"/>
+      <tableStyleElement type="firstRowSubheading" dxfId="10"/>
+      <tableStyleElement type="secondRowSubheading" dxfId="9"/>
+      <tableStyleElement type="pageFieldLabels" dxfId="8"/>
+      <tableStyleElement type="pageFieldValues" dxfId="7"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -876,7 +987,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1133,15 +1244,19 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="7" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="9.44444444444444" customWidth="1"/>
+    <col min="2" max="10" width="10.5555555555556" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1163,170 +1278,274 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:10">
       <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" t="s">
+      <c r="H2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" t="s">
+      <c r="I2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" t="s">
+      <c r="J2" t="s">
         <v>10</v>
       </c>
-      <c r="E2" t="s">
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J3" t="s">
         <v>11</v>
       </c>
-      <c r="F2" t="s">
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I4" t="s">
+        <v>11</v>
+      </c>
+      <c r="J4" t="s">
         <v>12</v>
       </c>
-      <c r="G2" t="s">
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I5" t="s">
+        <v>12</v>
+      </c>
+      <c r="J5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
-      <c r="A3" t="s">
+    <row r="6" spans="1:10">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" t="s">
+        <v>11</v>
+      </c>
+      <c r="H6" t="s">
+        <v>12</v>
+      </c>
+      <c r="I6" t="s">
+        <v>13</v>
+      </c>
+      <c r="J6" t="s">
         <v>14</v>
       </c>
-      <c r="B3" t="s">
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G7" t="s">
+        <v>12</v>
+      </c>
+      <c r="H7" t="s">
+        <v>13</v>
+      </c>
+      <c r="I7" t="s">
+        <v>14</v>
+      </c>
+      <c r="J7" t="s">
         <v>15</v>
       </c>
-      <c r="C3" t="s">
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H8" t="s">
+        <v>14</v>
+      </c>
+      <c r="I8" t="s">
+        <v>15</v>
+      </c>
+      <c r="J8" t="s">
         <v>16</v>
       </c>
-      <c r="D3" t="s">
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" t="s">
+        <v>13</v>
+      </c>
+      <c r="G9" t="s">
+        <v>14</v>
+      </c>
+      <c r="H9" t="s">
+        <v>15</v>
+      </c>
+      <c r="I9" t="s">
+        <v>16</v>
+      </c>
+      <c r="J9" t="s">
         <v>17</v>
-      </c>
-      <c r="E3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F3" t="s">
-        <v>19</v>
-      </c>
-      <c r="G3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D4" t="s">
-        <v>24</v>
-      </c>
-      <c r="E4" t="s">
-        <v>25</v>
-      </c>
-      <c r="F4" t="s">
-        <v>26</v>
-      </c>
-      <c r="G4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C5" t="s">
-        <v>30</v>
-      </c>
-      <c r="D5" t="s">
-        <v>31</v>
-      </c>
-      <c r="E5" t="s">
-        <v>32</v>
-      </c>
-      <c r="F5" t="s">
-        <v>33</v>
-      </c>
-      <c r="G5" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6" t="s">
-        <v>35</v>
-      </c>
-      <c r="B6" t="s">
-        <v>36</v>
-      </c>
-      <c r="C6" t="s">
-        <v>37</v>
-      </c>
-      <c r="D6" t="s">
-        <v>38</v>
-      </c>
-      <c r="E6" t="s">
-        <v>39</v>
-      </c>
-      <c r="F6" t="s">
-        <v>40</v>
-      </c>
-      <c r="G6" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="A7" t="s">
-        <v>42</v>
-      </c>
-      <c r="B7" t="s">
-        <v>43</v>
-      </c>
-      <c r="C7" t="s">
-        <v>44</v>
-      </c>
-      <c r="D7" t="s">
-        <v>45</v>
-      </c>
-      <c r="E7" t="s">
-        <v>46</v>
-      </c>
-      <c r="F7" t="s">
-        <v>47</v>
-      </c>
-      <c r="G7" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="A8" t="s">
-        <v>49</v>
-      </c>
-      <c r="B8" t="s">
-        <v>50</v>
-      </c>
-      <c r="C8" t="s">
-        <v>51</v>
-      </c>
-      <c r="D8" t="s">
-        <v>52</v>
-      </c>
-      <c r="E8" t="s">
-        <v>53</v>
-      </c>
-      <c r="F8" t="s">
-        <v>54</v>
-      </c>
-      <c r="G8" t="s">
-        <v>55</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
 </file>
@@ -1334,17 +1553,42 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A3"/>
+  <dimension ref="D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="2"/>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="5" outlineLevelCol="3"/>
   <sheetData>
-    <row r="3" spans="1:1">
-      <c r="A3" t="s">
-        <v>56</v>
+    <row r="6" spans="4:4">
+      <c r="D6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="10" defaultRowHeight="14.4" outlineLevelCol="1"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Read  and write excel data by column name
</commit_message>
<xml_diff>
--- a/TestData/New XLSX Worksheet.xlsx
+++ b/TestData/New XLSX Worksheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="22188" windowHeight="9000"/>
+    <workbookView windowWidth="20268" windowHeight="7920"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -29,9 +29,33 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="21">
-  <si>
-    <t>alsdfjdsf1</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="29">
+  <si>
+    <t>DFSDF</t>
+  </si>
+  <si>
+    <t>SDFEWR</t>
+  </si>
+  <si>
+    <t>SDFWER</t>
+  </si>
+  <si>
+    <t>WERDSF</t>
+  </si>
+  <si>
+    <t>WEWW</t>
+  </si>
+  <si>
+    <t>DSFXCCXZ</t>
+  </si>
+  <si>
+    <t>ZXCSD</t>
+  </si>
+  <si>
+    <t>TRYTHG</t>
+  </si>
+  <si>
+    <t>DSFSDF</t>
   </si>
   <si>
     <t>alsdfjdsf2</t>
@@ -1247,7 +1271,7 @@
   <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4"/>
@@ -1285,263 +1309,263 @@
         <v>8</v>
       </c>
       <c r="J1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="D2" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="E2" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="F2" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="G2" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="H2" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="I2" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="J2" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="D3" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="E3" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="F3" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="G3" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="H3" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="I3" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="J3" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="E4" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="F4" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="G4" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="H4" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="I4" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="J4" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="C5" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="D5" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="E5" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="F5" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="G5" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="H5" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="I5" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="J5" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="C6" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="D6" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="E6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F6" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="G6" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="H6" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="I6" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="J6" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="C7" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="D7" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E7" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="F7" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="G7" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="H7" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="I7" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="J7" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="B8" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="C8" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="D8" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="E8" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="F8" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="G8" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="H8" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="I8" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="J8" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:10">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="B9" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="C9" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="D9" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="E9" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="F9" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="G9" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="H9" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="I9" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="J9" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -1563,7 +1587,7 @@
   <sheetData>
     <row r="6" spans="4:4">
       <c r="D6" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -1585,10 +1609,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="B1" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>